<commit_message>
Added remaining cases; added ui for noun declensions; Folder restructuring;
</commit_message>
<xml_diff>
--- a/verbs.xlsx
+++ b/verbs.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VladimirNedoroslev\RiderProjects\open-kyrgyz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE0C65A-24F0-4FEE-AB61-C694F59C27F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0818F937-F91D-4F41-BED1-ED963083F05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="-уу" sheetId="3" r:id="rId1"/>
-    <sheet name="-үү" sheetId="1" r:id="rId2"/>
-    <sheet name="-оо" sheetId="2" r:id="rId3"/>
+    <sheet name="-оо" sheetId="2" r:id="rId2"/>
+    <sheet name="-үү" sheetId="1" r:id="rId3"/>
     <sheet name="-өө" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -1157,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C076EA17-3BFA-4F8E-B4D5-848155754FAD}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1652,15 +1652,227 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FE57FB-4179-4C54-B8C5-058760FA643D}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F3" t="s">
+        <v>244</v>
+      </c>
+      <c r="G3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>155</v>
+      </c>
+      <c r="B10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>194</v>
+      </c>
+      <c r="B11" t="s">
+        <v>193</v>
+      </c>
+      <c r="C11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12" t="s">
+        <v>203</v>
+      </c>
+      <c r="C12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>221</v>
+      </c>
+      <c r="B13" t="s">
+        <v>220</v>
+      </c>
+      <c r="C13" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>230</v>
+      </c>
+      <c r="B14" t="s">
+        <v>229</v>
+      </c>
+      <c r="C14" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>247</v>
+      </c>
+      <c r="B15" t="s">
+        <v>248</v>
+      </c>
+      <c r="C15" t="s">
+        <v>249</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1962,222 +2174,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FE57FB-4179-4C54-B8C5-058760FA643D}">
-  <dimension ref="A1:G15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F1" t="s">
-        <v>158</v>
-      </c>
-      <c r="G1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2" t="s">
-        <v>161</v>
-      </c>
-      <c r="F2" t="s">
-        <v>160</v>
-      </c>
-      <c r="G2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" t="s">
-        <v>245</v>
-      </c>
-      <c r="F3" t="s">
-        <v>244</v>
-      </c>
-      <c r="G3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B8" t="s">
-        <v>115</v>
-      </c>
-      <c r="C8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>155</v>
-      </c>
-      <c r="B10" t="s">
-        <v>156</v>
-      </c>
-      <c r="C10" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>194</v>
-      </c>
-      <c r="B11" t="s">
-        <v>193</v>
-      </c>
-      <c r="C11" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>202</v>
-      </c>
-      <c r="B12" t="s">
-        <v>203</v>
-      </c>
-      <c r="C12" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>221</v>
-      </c>
-      <c r="B13" t="s">
-        <v>220</v>
-      </c>
-      <c r="C13" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>230</v>
-      </c>
-      <c r="B14" t="s">
-        <v>229</v>
-      </c>
-      <c r="C14" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>247</v>
-      </c>
-      <c r="B15" t="s">
-        <v>248</v>
-      </c>
-      <c r="C15" t="s">
-        <v>249</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF691E14-A614-4633-AF78-FEEA8A0B7165}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2228,5 +2230,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>